<commit_message>
move code into Src folder
</commit_message>
<xml_diff>
--- a/Docs/Properites.xlsx
+++ b/Docs/Properites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jason\Gitee_Repos\ViaProjects\Tools\QAToolKit\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jason\Github_Repos\LiteToolSuite\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D59C7-1690-4BBF-A347-A475AF7F9EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B5B097-FBDD-48E9-BB30-049E78C228CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9390" yWindow="8055" windowWidth="29265" windowHeight="18510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12090" yWindow="6945" windowWidth="29265" windowHeight="18510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResXResourceManager" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Project</t>
   </si>
@@ -45,12 +45,99 @@
     <t>.zh-CN</t>
   </si>
   <si>
-    <t>QAToolKit</t>
+    <t>LiteToolSuite</t>
   </si>
   <si>
     <t>Properties\Resources</t>
   </si>
   <si>
+    <t>Feature1</t>
+  </si>
+  <si>
+    <t>MQTT消息</t>
+  </si>
+  <si>
+    <t>MQTT Message</t>
+  </si>
+  <si>
+    <t>Feature2</t>
+  </si>
+  <si>
+    <t>Feature3</t>
+  </si>
+  <si>
+    <t>文件改名</t>
+  </si>
+  <si>
+    <t>Rename</t>
+  </si>
+  <si>
+    <t>Feature4</t>
+  </si>
+  <si>
+    <t>时间/时间戳</t>
+  </si>
+  <si>
+    <t>Time/Timestamp</t>
+  </si>
+  <si>
+    <t>Feature5</t>
+  </si>
+  <si>
+    <t>车辆查看</t>
+  </si>
+  <si>
+    <t>Vehicle Configuration</t>
+  </si>
+  <si>
+    <t>Feature7</t>
+  </si>
+  <si>
+    <t>登录后端站点</t>
+  </si>
+  <si>
+    <t>Sign in Backend Site</t>
+  </si>
+  <si>
+    <t>登录后端l站点</t>
+  </si>
+  <si>
+    <t>Feature8</t>
+  </si>
+  <si>
+    <t>关于</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Feature9</t>
+  </si>
+  <si>
+    <t>退出程序</t>
+  </si>
+  <si>
+    <t>Exit QA ToolKit</t>
+  </si>
+  <si>
+    <t>MessageBoxCapInformation</t>
+  </si>
+  <si>
+    <t>提示</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>PhoneNumberPrompt</t>
+  </si>
+  <si>
+    <t>请输入11位手机号码</t>
+  </si>
+  <si>
+    <t>Please input 11 digital phone number</t>
+  </si>
+  <si>
     <t>PopMessage</t>
   </si>
   <si>
@@ -60,111 +147,16 @@
     <t>This is English!</t>
   </si>
   <si>
-    <t>Feature1</t>
-  </si>
-  <si>
-    <t>上传Log</t>
-  </si>
-  <si>
-    <t>Upload Debug Log</t>
-  </si>
-  <si>
-    <t>Feature2</t>
-  </si>
-  <si>
-    <t>MQTT订阅</t>
-  </si>
-  <si>
-    <t>MQTT Message</t>
-  </si>
-  <si>
-    <t>Feature3</t>
-  </si>
-  <si>
-    <t>查看Quota</t>
-  </si>
-  <si>
-    <t>Quota Detail</t>
-  </si>
-  <si>
-    <t>Feature4</t>
-  </si>
-  <si>
-    <t>周期拍照</t>
-  </si>
-  <si>
-    <t>Capture Camera Pics</t>
-  </si>
-  <si>
-    <t>Feature5</t>
-  </si>
-  <si>
-    <t>车辆查看</t>
-  </si>
-  <si>
-    <t>Vehicle Configuration</t>
+    <t>SearchTextPrompt</t>
+  </si>
+  <si>
+    <t>请输入搜索内容</t>
+  </si>
+  <si>
+    <t>Please input search text</t>
   </si>
   <si>
     <t>Feature6</t>
-  </si>
-  <si>
-    <t>时间/时间戳</t>
-  </si>
-  <si>
-    <t>Time/Timestamp</t>
-  </si>
-  <si>
-    <t>时间时间戳</t>
-  </si>
-  <si>
-    <t>Feature7</t>
-  </si>
-  <si>
-    <t>登录Serverful站点</t>
-  </si>
-  <si>
-    <t>Sign In Serverful</t>
-  </si>
-  <si>
-    <t>Feature8</t>
-  </si>
-  <si>
-    <t>关于</t>
-  </si>
-  <si>
-    <t>About</t>
-  </si>
-  <si>
-    <t>Feature9</t>
-  </si>
-  <si>
-    <t>退出程序</t>
-  </si>
-  <si>
-    <t>Exit QA ToolKit</t>
-  </si>
-  <si>
-    <t>PhoneNumberPrompt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请输入11位手机号码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Please input 11 digital phone number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SerachTextPrompt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请输入搜索内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Please input search text</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,19 +519,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
-    <col min="3" max="3" width="28.375" customWidth="1"/>
-    <col min="4" max="4" width="25.125" customWidth="1"/>
-    <col min="5" max="5" width="31.375" customWidth="1"/>
-    <col min="6" max="6" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="28.625" customWidth="1"/>
+    <col min="4" max="4" width="40.75" customWidth="1"/>
+    <col min="5" max="5" width="85.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -593,13 +583,13 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -610,16 +600,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -630,16 +620,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -650,16 +640,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -670,16 +660,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -690,16 +671,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -710,16 +682,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -730,16 +702,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -750,56 +722,76 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>43</v>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>